<commit_message>
ccdc test scripts and copy of 100fix fm develop branch
</commit_message>
<xml_diff>
--- a/InputFiles/CCDC_ParticipatingResources.xlsx
+++ b/InputFiles/CCDC_ParticipatingResources.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D145AB9-E23B-4EF7-9A02-35DEC6ED0AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ResourceDetailed" sheetId="1" r:id="rId1"/>
+    <sheet name="ResourcePage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +25,385 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="124">
+  <si>
+    <t>CGCI</t>
+  </si>
+  <si>
+    <t>suffixUrl</t>
+  </si>
+  <si>
+    <t>/resource/CGC</t>
+  </si>
+  <si>
+    <t>/resource/CGCI</t>
+  </si>
+  <si>
+    <t>CGC</t>
+  </si>
+  <si>
+    <t>ResourceName</t>
+  </si>
+  <si>
+    <t>ResourceCode</t>
+  </si>
+  <si>
+    <t>Cancer Genomics Cloud</t>
+  </si>
+  <si>
+    <t>Cancer Genome Characterization Initiative</t>
+  </si>
+  <si>
+    <t>FilterType</t>
+  </si>
+  <si>
+    <t>DtstSummaryCnt</t>
+  </si>
+  <si>
+    <t>PROGRAM</t>
+  </si>
+  <si>
+    <t>ANALYTIC TOOL</t>
+  </si>
+  <si>
+    <t>HTAN</t>
+  </si>
+  <si>
+    <t>Center for Pediatric Tumor Cell Atlas</t>
+  </si>
+  <si>
+    <t>/resource/HTAN</t>
+  </si>
+  <si>
+    <t>Central Brain Tumor Registry of the United States</t>
+  </si>
+  <si>
+    <t>CBTRUS</t>
+  </si>
+  <si>
+    <t>/resource/CBTRUS</t>
+  </si>
+  <si>
+    <t>REGISTRY</t>
+  </si>
+  <si>
+    <t>/resource/CLIC</t>
+  </si>
+  <si>
+    <t>Childhood Cancer &amp; Leukemia International Consortium</t>
+  </si>
+  <si>
+    <t>CLIC</t>
+  </si>
+  <si>
+    <t>CATALOG</t>
+  </si>
+  <si>
+    <t>Childhood Cancer Data Initiative</t>
+  </si>
+  <si>
+    <t>/resource/CCDI</t>
+  </si>
+  <si>
+    <t>CCDI</t>
+  </si>
+  <si>
+    <t>/resource/CCSS</t>
+  </si>
+  <si>
+    <t>Childhood Cancer Survivor Study</t>
+  </si>
+  <si>
+    <t>CCSS</t>
+  </si>
+  <si>
+    <t>Children's Oncology Group</t>
+  </si>
+  <si>
+    <t>/resource/COG</t>
+  </si>
+  <si>
+    <t>COG</t>
+  </si>
+  <si>
+    <t>Clinical Interpretations of Variants in Cancer</t>
+  </si>
+  <si>
+    <t>KNOWLEDGEBASE</t>
+  </si>
+  <si>
+    <t>/resource/GEO</t>
+  </si>
+  <si>
+    <t>Gene Expression Omnibus</t>
+  </si>
+  <si>
+    <t>GEO</t>
+  </si>
+  <si>
+    <t>REPOSITORY</t>
+  </si>
+  <si>
+    <t>/resource/GDC</t>
+  </si>
+  <si>
+    <t>Genomic Data Commons</t>
+  </si>
+  <si>
+    <t>GDC</t>
+  </si>
+  <si>
+    <t>/resource/HitWalker2</t>
+  </si>
+  <si>
+    <t>HitWalker2</t>
+  </si>
+  <si>
+    <t>/resource/HCMI</t>
+  </si>
+  <si>
+    <t>Human Cancer Models Initiative</t>
+  </si>
+  <si>
+    <t>HCMI</t>
+  </si>
+  <si>
+    <t>/resource/iCat</t>
+  </si>
+  <si>
+    <t>Individualized Cancer Therapy Study</t>
+  </si>
+  <si>
+    <t>iCat</t>
+  </si>
+  <si>
+    <t>PROJECT</t>
+  </si>
+  <si>
+    <t>International Cancer Genome Consortium</t>
+  </si>
+  <si>
+    <t>/resource/ICGC</t>
+  </si>
+  <si>
+    <t>ICGC</t>
+  </si>
+  <si>
+    <t>Kids First Data Resource</t>
+  </si>
+  <si>
+    <t>/resource/Kids%20First%20Data%20Resource</t>
+  </si>
+  <si>
+    <t>MicroRNA Childhood Cancer Catalog</t>
+  </si>
+  <si>
+    <t>/resource/M3Cs</t>
+  </si>
+  <si>
+    <t>M3Cs</t>
+  </si>
+  <si>
+    <t>Molecular Targets Platform</t>
+  </si>
+  <si>
+    <t>/resource/MTP</t>
+  </si>
+  <si>
+    <t>MTP</t>
+  </si>
+  <si>
+    <t>/resource/MyPART</t>
+  </si>
+  <si>
+    <t>MyPART</t>
+  </si>
+  <si>
+    <t>National Childhood Cancer Registry Explorer</t>
+  </si>
+  <si>
+    <t>/resource/NCCR</t>
+  </si>
+  <si>
+    <t>NCCR</t>
+  </si>
+  <si>
+    <t>/resource/Oncogenomics</t>
+  </si>
+  <si>
+    <t>Oncogenomics</t>
+  </si>
+  <si>
+    <t>/resource/OncoKB</t>
+  </si>
+  <si>
+    <t>OncoKB</t>
+  </si>
+  <si>
+    <t>Patient-Derived Xenograft and Advanced In Vivo Models</t>
+  </si>
+  <si>
+    <t>/resource/PDX%20AIM</t>
+  </si>
+  <si>
+    <t>PDX AIM</t>
+  </si>
+  <si>
+    <t>PDX Development and Trial Centers Research Network</t>
+  </si>
+  <si>
+    <t>/resource/PDXNet</t>
+  </si>
+  <si>
+    <t>PDXNet</t>
+  </si>
+  <si>
+    <t>PDX for Childhood Cancer Therapeutics</t>
+  </si>
+  <si>
+    <t>/resource/PCAT</t>
+  </si>
+  <si>
+    <t>PCAT</t>
+  </si>
+  <si>
+    <t>PedcBioPortal for Integrated Childhood Cancer Genomics</t>
+  </si>
+  <si>
+    <t>/resource/PEDC</t>
+  </si>
+  <si>
+    <t>PEDC</t>
+  </si>
+  <si>
+    <t>/resource/PCDC</t>
+  </si>
+  <si>
+    <t>Pediatric Cancer Data Commons</t>
+  </si>
+  <si>
+    <t>PCDC</t>
+  </si>
+  <si>
+    <t>Pediatric MATCH</t>
+  </si>
+  <si>
+    <t>/resource/PedMATCH</t>
+  </si>
+  <si>
+    <t>PedMATCH</t>
+  </si>
+  <si>
+    <t>/resource/PPTC</t>
+  </si>
+  <si>
+    <t>Pediatric Preclinical Testing Consortium</t>
+  </si>
+  <si>
+    <t>PPTC</t>
+  </si>
+  <si>
+    <t>Population-based Research to Optimize the Screening Process</t>
+  </si>
+  <si>
+    <t>/resource/PROSPR</t>
+  </si>
+  <si>
+    <t>PROSPR</t>
+  </si>
+  <si>
+    <t>Single-cell Pediatric Cancer Atlas</t>
+  </si>
+  <si>
+    <t>/resource/ScPCA</t>
+  </si>
+  <si>
+    <t>ScPCA</t>
+  </si>
+  <si>
+    <t>St. Jude Cloud</t>
+  </si>
+  <si>
+    <t>/resource/St.%20Jude%20Cloud</t>
+  </si>
+  <si>
+    <t>Texas KidsCanSeq</t>
+  </si>
+  <si>
+    <t>/resource/Texas%20KidsCanSeq</t>
+  </si>
+  <si>
+    <t>/resource/TCIA</t>
+  </si>
+  <si>
+    <t>TCIA</t>
+  </si>
+  <si>
+    <t>The Cancer Imaging Archive</t>
+  </si>
+  <si>
+    <t>The database of Genotypes and Phenotypes</t>
+  </si>
+  <si>
+    <t>dbGaP</t>
+  </si>
+  <si>
+    <t>/resource/dbGaP</t>
+  </si>
+  <si>
+    <t>The Jackson Laboratory PDX Models</t>
+  </si>
+  <si>
+    <t>JAX PDX</t>
+  </si>
+  <si>
+    <t>/resource/JAX%20PDX</t>
+  </si>
+  <si>
+    <t>Therapeutically Applicable Research To Generate Effective Treatments</t>
+  </si>
+  <si>
+    <t>/resource/TARGET</t>
+  </si>
+  <si>
+    <t>TARGET</t>
+  </si>
+  <si>
+    <t>Treehouse Childhood Cancer Initiative</t>
+  </si>
+  <si>
+    <t>/resource/Treehouse</t>
+  </si>
+  <si>
+    <t>Treehouse</t>
+  </si>
+  <si>
+    <t>Victorian Paediatric Cancer Consortium</t>
+  </si>
+  <si>
+    <t>/resource/VPCC</t>
+  </si>
+  <si>
+    <t>VPCC</t>
+  </si>
+  <si>
+    <t>/resource/Vizome</t>
+  </si>
+  <si>
+    <t>Vizome</t>
+  </si>
+  <si>
+    <t>CIViC</t>
+  </si>
+  <si>
+    <t>/resource/CIViC</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +714,777 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE648D8-28E6-4A29-9364-DDD9BB85DA09}">
+  <dimension ref="A1:E41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>93</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36">
+        <v>54</v>
+      </c>
+      <c r="E36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" t="s">
+        <v>116</v>
+      </c>
+      <c r="D39">
+        <v>8</v>
+      </c>
+      <c r="E39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" t="s">
+        <v>117</v>
+      </c>
+      <c r="C40" t="s">
+        <v>119</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" t="s">
+        <v>121</v>
+      </c>
+      <c r="C41" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ccdc datasets and resources
</commit_message>
<xml_diff>
--- a/InputFiles/CCDC_ParticipatingResources.xlsx
+++ b/InputFiles/CCDC_ParticipatingResources.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\March\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\April\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815D93F4-94D9-41E3-9D8D-9494835081B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995EE062-6F86-4B22-AC25-B2C166222F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ResourcePage" sheetId="2" r:id="rId1"/>
@@ -411,33 +411,33 @@
     <t>Program</t>
   </si>
   <si>
-    <t>Data Update Date</t>
-  </si>
-  <si>
-    <t>Visualization Tools</t>
-  </si>
-  <si>
-    <t>Analytic Tools</t>
-  </si>
-  <si>
-    <t>Data Content Type</t>
-  </si>
-  <si>
     <t xml:space="preserve">
 Genomics/Omics, Imaging, Clinical</t>
   </si>
   <si>
-    <t>Point of Contact</t>
-  </si>
-  <si>
     <t>Office of Cancer Genomics</t>
+  </si>
+  <si>
+    <t>PointOfContact</t>
+  </si>
+  <si>
+    <t>DataUpdateDate</t>
+  </si>
+  <si>
+    <t>VisualizationTools</t>
+  </si>
+  <si>
+    <t>AnalyticTools</t>
+  </si>
+  <si>
+    <t>DataContentType</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,13 +445,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6E6E6E"/>
+        <bgColor rgb="FF6E6E6E"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -466,12 +478,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,60 +768,60 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>124</v>
-      </c>
-      <c r="H1" t="s">
-        <v>125</v>
-      </c>
-      <c r="I1" t="s">
-        <v>128</v>
-      </c>
-      <c r="J1" t="s">
-        <v>129</v>
-      </c>
-      <c r="K1" t="s">
-        <v>130</v>
-      </c>
-      <c r="L1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="L1" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -819,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -837,10 +850,10 @@
         <v>44747</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -857,7 +870,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -874,7 +887,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -891,7 +904,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -908,7 +921,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -925,7 +938,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -942,7 +955,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -959,7 +972,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -976,7 +989,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -993,7 +1006,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1010,7 +1023,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1027,7 +1040,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -1044,7 +1057,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1061,7 +1074,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -1078,7 +1091,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1095,7 +1108,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -1112,7 +1125,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -1129,7 +1142,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -1146,7 +1159,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>65</v>
       </c>
@@ -1163,7 +1176,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -1180,7 +1193,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -1197,7 +1210,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>72</v>
       </c>
@@ -1214,7 +1227,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>75</v>
       </c>
@@ -1231,7 +1244,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>78</v>
       </c>
@@ -1248,7 +1261,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -1265,7 +1278,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>83</v>
       </c>
@@ -1282,7 +1295,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>87</v>
       </c>
@@ -1299,7 +1312,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>89</v>
       </c>
@@ -1316,7 +1329,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>93</v>
       </c>
@@ -1333,7 +1346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>96</v>
       </c>
@@ -1350,7 +1363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>99</v>
       </c>
@@ -1367,7 +1380,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>101</v>
       </c>
@@ -1384,7 +1397,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>102</v>
       </c>
@@ -1401,7 +1414,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>107</v>
       </c>
@@ -1418,7 +1431,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -1435,7 +1448,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -1452,7 +1465,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>115</v>
       </c>
@@ -1469,7 +1482,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>118</v>
       </c>
@@ -1486,7 +1499,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>120</v>
       </c>

</xml_diff>